<commit_message>
Adding files from last week's lab on creating a visual search experiment
</commit_message>
<xml_diff>
--- a/Cog Sci 242 F17 Lab 6 - Regression Analysis My Data.xlsx
+++ b/Cog Sci 242 F17 Lab 6 - Regression Analysis My Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanessa5\Google Drive\Oxy 2018 Fall\CogS 242\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1797E1AB-6CAE-4E83-8C9E-47236B23BF5A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03107AC-F07D-41B4-AFFC-DE885E298EC5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1343" windowWidth="25283" windowHeight="13523" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1343" windowWidth="25283" windowHeight="13523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="15" r:id="rId1"/>
@@ -2191,7 +2191,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2235,7 +2235,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2259,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5797,7 +5797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -6775,7 +6775,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
-        <f>IF(COUNTBLANK(C28)=0,A27+1,A27)</f>
+        <f t="shared" ref="A28:A36" si="9">IF(COUNTBLANK(C28)=0,A27+1,A27)</f>
         <v>15</v>
       </c>
       <c r="B28" s="3">
@@ -6785,27 +6785,27 @@
         <v>859</v>
       </c>
       <c r="D28" s="36">
-        <f>IF(COUNTBLANK(B28)=0,$D$3," ")</f>
+        <f t="shared" ref="D28:D36" si="10">IF(COUNTBLANK(B28)=0,$D$3," ")</f>
         <v>1015.7142857142857</v>
       </c>
       <c r="E28" s="37">
-        <f>IF(COUNTBLANK(B28)=0,C28-D28," ")</f>
+        <f t="shared" ref="E28:E36" si="11">IF(COUNTBLANK(B28)=0,C28-D28," ")</f>
         <v>-156.71428571428567</v>
       </c>
       <c r="F28" s="37">
-        <f>IF(COUNTBLANK(B28)=0,E28*E28," ")</f>
+        <f t="shared" ref="F28:F36" si="12">IF(COUNTBLANK(B28)=0,E28*E28," ")</f>
         <v>24559.367346938761</v>
       </c>
       <c r="G28" s="38">
-        <f>IF(COUNTBLANK(B28) = 0, $D$5*B28+$F$5," ")</f>
+        <f t="shared" ref="G28:G36" si="13">IF(COUNTBLANK(B28) = 0, $D$5*B28+$F$5," ")</f>
         <v>1470.0612244897957</v>
       </c>
       <c r="H28" s="39">
-        <f>IF(COUNTBLANK(B28)=0,C28-G28," ")</f>
+        <f t="shared" ref="H28:H36" si="14">IF(COUNTBLANK(B28)=0,C28-G28," ")</f>
         <v>-611.06122448979568</v>
       </c>
       <c r="I28" s="39">
-        <f>IF(COUNTBLANK(B28)=0, H28*H28," ")</f>
+        <f t="shared" ref="I28:I36" si="15">IF(COUNTBLANK(B28)=0, H28*H28," ")</f>
         <v>373395.82007496845</v>
       </c>
       <c r="R28" s="3">
@@ -6819,7 +6819,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
-        <f>IF(COUNTBLANK(C29)=0,A28+1,A28)</f>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="B29" s="3">
@@ -6829,27 +6829,27 @@
         <v>1347</v>
       </c>
       <c r="D29" s="36">
-        <f>IF(COUNTBLANK(B29)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E29" s="37">
-        <f>IF(COUNTBLANK(B29)=0,C29-D29," ")</f>
+        <f t="shared" si="11"/>
         <v>331.28571428571433</v>
       </c>
       <c r="F29" s="37">
-        <f>IF(COUNTBLANK(B29)=0,E29*E29," ")</f>
+        <f t="shared" si="12"/>
         <v>109750.22448979595</v>
       </c>
       <c r="G29" s="38">
-        <f>IF(COUNTBLANK(B29) = 0, $D$5*B29+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H29" s="39">
-        <f>IF(COUNTBLANK(B29)=0,C29-G29," ")</f>
+        <f t="shared" si="14"/>
         <v>-123.06122448979568</v>
       </c>
       <c r="I29" s="39">
-        <f>IF(COUNTBLANK(B29)=0, H29*H29," ")</f>
+        <f t="shared" si="15"/>
         <v>15144.064972927887</v>
       </c>
       <c r="K29" s="69"/>
@@ -6857,17 +6857,17 @@
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
       <c r="R29" s="3">
-        <f>IF(COUNTBLANK(B28)=0,B28*B28," ")</f>
+        <f t="shared" ref="R29:R37" si="16">IF(COUNTBLANK(B28)=0,B28*B28," ")</f>
         <v>4096</v>
       </c>
       <c r="S29" s="3">
-        <f>IF(COUNTBLANK(B28)=0,B28*C28," ")</f>
+        <f t="shared" ref="S29:S37" si="17">IF(COUNTBLANK(B28)=0,B28*C28," ")</f>
         <v>54976</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
-        <f>IF(COUNTBLANK(C30)=0,A29+1,A29)</f>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B30" s="3">
@@ -6877,27 +6877,27 @@
         <v>1355</v>
       </c>
       <c r="D30" s="36">
-        <f>IF(COUNTBLANK(B30)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E30" s="37">
-        <f>IF(COUNTBLANK(B30)=0,C30-D30," ")</f>
+        <f t="shared" si="11"/>
         <v>339.28571428571433</v>
       </c>
       <c r="F30" s="37">
-        <f>IF(COUNTBLANK(B30)=0,E30*E30," ")</f>
+        <f t="shared" si="12"/>
         <v>115114.79591836738</v>
       </c>
       <c r="G30" s="38">
-        <f>IF(COUNTBLANK(B30) = 0, $D$5*B30+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H30" s="39">
-        <f>IF(COUNTBLANK(B30)=0,C30-G30," ")</f>
+        <f t="shared" si="14"/>
         <v>-115.06122448979568</v>
       </c>
       <c r="I30" s="39">
-        <f>IF(COUNTBLANK(B30)=0, H30*H30," ")</f>
+        <f t="shared" si="15"/>
         <v>13239.085381091156</v>
       </c>
       <c r="K30" s="69"/>
@@ -6905,17 +6905,17 @@
       <c r="M30" s="69"/>
       <c r="N30" s="69"/>
       <c r="R30" s="3">
-        <f>IF(COUNTBLANK(B29)=0,B29*B29," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S30" s="3">
-        <f>IF(COUNTBLANK(B29)=0,B29*C29," ")</f>
+        <f t="shared" si="17"/>
         <v>86208</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
-        <f>IF(COUNTBLANK(C31)=0,A30+1,A30)</f>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="B31" s="3">
@@ -6925,41 +6925,41 @@
         <v>1414</v>
       </c>
       <c r="D31" s="36">
-        <f>IF(COUNTBLANK(B31)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E31" s="37">
-        <f>IF(COUNTBLANK(B31)=0,C31-D31," ")</f>
+        <f t="shared" si="11"/>
         <v>398.28571428571433</v>
       </c>
       <c r="F31" s="37">
-        <f>IF(COUNTBLANK(B31)=0,E31*E31," ")</f>
+        <f t="shared" si="12"/>
         <v>158631.51020408169</v>
       </c>
       <c r="G31" s="38">
-        <f>IF(COUNTBLANK(B31) = 0, $D$5*B31+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H31" s="39">
-        <f>IF(COUNTBLANK(B31)=0,C31-G31," ")</f>
+        <f t="shared" si="14"/>
         <v>-56.061224489795677</v>
       </c>
       <c r="I31" s="39">
-        <f>IF(COUNTBLANK(B31)=0, H31*H31," ")</f>
+        <f t="shared" si="15"/>
         <v>3142.8608912952664</v>
       </c>
       <c r="R31" s="3">
-        <f>IF(COUNTBLANK(B30)=0,B30*B30," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S31" s="3">
-        <f>IF(COUNTBLANK(B30)=0,B30*C30," ")</f>
+        <f t="shared" si="17"/>
         <v>86720</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
-        <f>IF(COUNTBLANK(C32)=0,A31+1,A31)</f>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="B32" s="3">
@@ -6969,41 +6969,41 @@
         <v>1452</v>
       </c>
       <c r="D32" s="36">
-        <f>IF(COUNTBLANK(B32)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E32" s="37">
-        <f>IF(COUNTBLANK(B32)=0,C32-D32," ")</f>
+        <f t="shared" si="11"/>
         <v>436.28571428571433</v>
       </c>
       <c r="F32" s="37">
-        <f>IF(COUNTBLANK(B32)=0,E32*E32," ")</f>
+        <f t="shared" si="12"/>
         <v>190345.22448979598</v>
       </c>
       <c r="G32" s="38">
-        <f>IF(COUNTBLANK(B32) = 0, $D$5*B32+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H32" s="39">
-        <f>IF(COUNTBLANK(B32)=0,C32-G32," ")</f>
+        <f t="shared" si="14"/>
         <v>-18.061224489795677</v>
       </c>
       <c r="I32" s="39">
-        <f>IF(COUNTBLANK(B32)=0, H32*H32," ")</f>
+        <f t="shared" si="15"/>
         <v>326.20783007079513</v>
       </c>
       <c r="R32" s="3">
-        <f>IF(COUNTBLANK(B31)=0,B31*B31," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S32" s="3">
-        <f>IF(COUNTBLANK(B31)=0,B31*C31," ")</f>
+        <f t="shared" si="17"/>
         <v>90496</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
-        <f>IF(COUNTBLANK(C33)=0,A32+1,A32)</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="B33" s="3">
@@ -7013,41 +7013,41 @@
         <v>1662</v>
       </c>
       <c r="D33" s="36">
-        <f>IF(COUNTBLANK(B33)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E33" s="37">
-        <f>IF(COUNTBLANK(B33)=0,C33-D33," ")</f>
+        <f t="shared" si="11"/>
         <v>646.28571428571433</v>
       </c>
       <c r="F33" s="37">
-        <f>IF(COUNTBLANK(B33)=0,E33*E33," ")</f>
+        <f t="shared" si="12"/>
         <v>417685.22448979598</v>
       </c>
       <c r="G33" s="38">
-        <f>IF(COUNTBLANK(B33) = 0, $D$5*B33+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H33" s="39">
-        <f>IF(COUNTBLANK(B33)=0,C33-G33," ")</f>
+        <f t="shared" si="14"/>
         <v>191.93877551020432</v>
       </c>
       <c r="I33" s="39">
-        <f>IF(COUNTBLANK(B33)=0, H33*H33," ")</f>
+        <f t="shared" si="15"/>
         <v>36840.493544356614</v>
       </c>
       <c r="R33" s="3">
-        <f>IF(COUNTBLANK(B32)=0,B32*B32," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S33" s="3">
-        <f>IF(COUNTBLANK(B32)=0,B32*C32," ")</f>
+        <f t="shared" si="17"/>
         <v>92928</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
-        <f>IF(COUNTBLANK(C34)=0,A33+1,A33)</f>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B34" s="3">
@@ -7057,115 +7057,115 @@
         <v>2039</v>
       </c>
       <c r="D34" s="36">
-        <f>IF(COUNTBLANK(B34)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v>1015.7142857142857</v>
       </c>
       <c r="E34" s="37">
-        <f>IF(COUNTBLANK(B34)=0,C34-D34," ")</f>
+        <f t="shared" si="11"/>
         <v>1023.2857142857143</v>
       </c>
       <c r="F34" s="37">
-        <f>IF(COUNTBLANK(B34)=0,E34*E34," ")</f>
+        <f t="shared" si="12"/>
         <v>1047113.6530612246</v>
       </c>
       <c r="G34" s="38">
-        <f>IF(COUNTBLANK(B34) = 0, $D$5*B34+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v>1470.0612244897957</v>
       </c>
       <c r="H34" s="39">
-        <f>IF(COUNTBLANK(B34)=0,C34-G34," ")</f>
+        <f t="shared" si="14"/>
         <v>568.93877551020432</v>
       </c>
       <c r="I34" s="39">
-        <f>IF(COUNTBLANK(B34)=0, H34*H34," ")</f>
+        <f t="shared" si="15"/>
         <v>323691.33027905069</v>
       </c>
       <c r="R34" s="3">
-        <f>IF(COUNTBLANK(B33)=0,B33*B33," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S34" s="3">
-        <f>IF(COUNTBLANK(B33)=0,B33*C33," ")</f>
+        <f t="shared" si="17"/>
         <v>106368</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
-        <f>IF(COUNTBLANK(C35)=0,A34+1,A34)</f>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="36" t="str">
-        <f>IF(COUNTBLANK(B35)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E35" s="37" t="str">
-        <f>IF(COUNTBLANK(B35)=0,C35-D35," ")</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F35" s="37" t="str">
-        <f>IF(COUNTBLANK(B35)=0,E35*E35," ")</f>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G35" s="38" t="str">
-        <f>IF(COUNTBLANK(B35) = 0, $D$5*B35+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H35" s="39" t="str">
-        <f>IF(COUNTBLANK(B35)=0,C35-G35," ")</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I35" s="39" t="str">
-        <f>IF(COUNTBLANK(B35)=0, H35*H35," ")</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R35" s="3">
-        <f>IF(COUNTBLANK(B34)=0,B34*B34," ")</f>
+        <f t="shared" si="16"/>
         <v>4096</v>
       </c>
       <c r="S35" s="3">
-        <f>IF(COUNTBLANK(B34)=0,B34*C34," ")</f>
+        <f t="shared" si="17"/>
         <v>130496</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
-        <f>IF(COUNTBLANK(C36)=0,A35+1,A35)</f>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="36" t="str">
-        <f>IF(COUNTBLANK(B36)=0,$D$3," ")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E36" s="37" t="str">
-        <f>IF(COUNTBLANK(B36)=0,C36-D36," ")</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F36" s="37" t="str">
-        <f>IF(COUNTBLANK(B36)=0,E36*E36," ")</f>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G36" s="38" t="str">
-        <f>IF(COUNTBLANK(B36) = 0, $D$5*B36+$F$5," ")</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H36" s="39" t="str">
-        <f>IF(COUNTBLANK(B36)=0,C36-G36," ")</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I36" s="39" t="str">
-        <f>IF(COUNTBLANK(B36)=0, H36*H36," ")</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R36" s="3" t="str">
-        <f>IF(COUNTBLANK(B35)=0,B35*B35," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S36" s="3" t="str">
-        <f>IF(COUNTBLANK(B35)=0,B35*C35," ")</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7201,11 +7201,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="R37" s="3" t="str">
-        <f>IF(COUNTBLANK(B36)=0,B36*B36," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S37" s="3" t="str">
-        <f>IF(COUNTBLANK(B36)=0,B36*C36," ")</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>

</xml_diff>